<commit_message>
Added another Two-Way ANOVA Problem
</commit_message>
<xml_diff>
--- a/ANOVA_using_excel/ANOVA_tests_using_excel.xlsx
+++ b/ANOVA_using_excel/ANOVA_tests_using_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\STUDY\Projects\Maths_for_ML\Statistics_for_ML\ANOVA_using_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F53280-A339-45D9-997C-557E16BE8BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379F71CD-79F4-4CB7-B6C0-7A22BA634FDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{A511CB45-DD40-48DB-BA89-DED05738D4E4}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="ANOVA 2-way Plants DS results" sheetId="15" r:id="rId6"/>
     <sheet name="Batsmen_Runs_Dataset" sheetId="18" r:id="rId7"/>
     <sheet name="ANOVA 2-way Batsmen results" sheetId="19" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="23" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="93">
   <si>
     <t>Sehwag</t>
   </si>
@@ -303,6 +304,21 @@
   <si>
     <t>TB</t>
   </si>
+  <si>
+    <t>PATIENT</t>
+  </si>
+  <si>
+    <t>BASELINE</t>
+  </si>
+  <si>
+    <t>GUM</t>
+  </si>
+  <si>
+    <t>MIN30</t>
+  </si>
+  <si>
+    <t>MIN60</t>
+  </si>
 </sst>
 </file>
 
@@ -397,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -486,11 +502,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -568,6 +599,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9214,9 +9251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89827569-FC2F-406C-AFC4-5B3A87E2491F}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9843,7 +9878,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A98851A-B4ED-4695-A3FB-2D9C2E64C310}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11074,10 +11111,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F878F53-0EBD-4E02-8090-6D10BAC03C0D}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11734,7 +11771,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>45</v>
       </c>
@@ -11756,8 +11793,16 @@
       <c r="G49" s="5">
         <v>2.4771686727109157</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49">
+        <f>B49/D49</f>
+        <v>5</v>
+      </c>
+      <c r="I49">
+        <f>_xlfn.F.INV.RT(0.05,5,36)</f>
+        <v>2.4771686727109157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>46</v>
       </c>
@@ -11779,8 +11824,12 @@
       <c r="G50" s="5">
         <v>3.2594463061441079</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I50">
+        <f>_xlfn.F.INV.RT(0.05,2,36)</f>
+        <v>3.2594463061441079</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>42</v>
       </c>
@@ -11802,8 +11851,12 @@
       <c r="G51" s="5">
         <v>2.1060539102611209</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I51">
+        <f>_xlfn.F.INV.RT(0.05,10,36)</f>
+        <v>2.1060539102611209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>57</v>
       </c>
@@ -11820,7 +11873,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -11828,8 +11881,12 @@
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
-    </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I53">
+        <f>_xlfn.F.INV.RT(0.01,9,27)</f>
+        <v>3.1493854106511754</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>27</v>
       </c>
@@ -13013,10 +13070,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CABFB07-753C-4C3C-96F8-72B8641F2CD1}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13262,7 +13319,7 @@
         <v>153.35714285714286</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>67</v>
       </c>
@@ -13279,12 +13336,12 @@
         <v>1173.0714285714287</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>33</v>
       </c>
@@ -13307,7 +13364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>73</v>
       </c>
@@ -13329,8 +13386,12 @@
       <c r="G22" s="5">
         <v>2.3592598540564387</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <f>_xlfn.F.INV.RT(0.05,2,8)</f>
+        <v>4.4589701075245118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>41</v>
       </c>
@@ -13353,7 +13414,7 @@
         <v>2.7140758041450779</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>74</v>
       </c>
@@ -13370,7 +13431,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -13379,7 +13440,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
@@ -13397,4 +13458,598 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1348DE27-F265-4030-8EEC-652A68ECEA46}">
+  <dimension ref="A1:M38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="33">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33">
+        <v>249</v>
+      </c>
+      <c r="C2" s="33">
+        <v>108</v>
+      </c>
+      <c r="D2" s="33">
+        <v>93</v>
+      </c>
+      <c r="E2" s="33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="33">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33">
+        <v>1095</v>
+      </c>
+      <c r="C3" s="33">
+        <v>593</v>
+      </c>
+      <c r="D3" s="33">
+        <v>600</v>
+      </c>
+      <c r="E3" s="33">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="33">
+        <v>3</v>
+      </c>
+      <c r="B4" s="33">
+        <v>83</v>
+      </c>
+      <c r="C4" s="33">
+        <v>27</v>
+      </c>
+      <c r="D4" s="33">
+        <v>32</v>
+      </c>
+      <c r="E4" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="33">
+        <v>4</v>
+      </c>
+      <c r="B5" s="33">
+        <v>569</v>
+      </c>
+      <c r="C5" s="33">
+        <v>363</v>
+      </c>
+      <c r="D5" s="33">
+        <v>342</v>
+      </c>
+      <c r="E5" s="33">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="33">
+        <v>5</v>
+      </c>
+      <c r="B6" s="33">
+        <v>368</v>
+      </c>
+      <c r="C6" s="33">
+        <v>141</v>
+      </c>
+      <c r="D6" s="33">
+        <v>167</v>
+      </c>
+      <c r="E6" s="33">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="33">
+        <v>6</v>
+      </c>
+      <c r="B7" s="33">
+        <v>326</v>
+      </c>
+      <c r="C7" s="33">
+        <v>134</v>
+      </c>
+      <c r="D7" s="33">
+        <v>144</v>
+      </c>
+      <c r="E7" s="33">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="33">
+        <v>7</v>
+      </c>
+      <c r="B8" s="33">
+        <v>324</v>
+      </c>
+      <c r="C8" s="33">
+        <v>126</v>
+      </c>
+      <c r="D8" s="33">
+        <v>312</v>
+      </c>
+      <c r="E8" s="33">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="33">
+        <v>8</v>
+      </c>
+      <c r="B9" s="33">
+        <v>95</v>
+      </c>
+      <c r="C9" s="33">
+        <v>41</v>
+      </c>
+      <c r="D9" s="33">
+        <v>63</v>
+      </c>
+      <c r="E9" s="33">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="33">
+        <v>9</v>
+      </c>
+      <c r="B10" s="33">
+        <v>413</v>
+      </c>
+      <c r="C10" s="33">
+        <v>365</v>
+      </c>
+      <c r="D10" s="33">
+        <v>282</v>
+      </c>
+      <c r="E10" s="33">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="33">
+        <v>10</v>
+      </c>
+      <c r="B11" s="33">
+        <v>332</v>
+      </c>
+      <c r="C11" s="33">
+        <v>293</v>
+      </c>
+      <c r="D11" s="33">
+        <v>525</v>
+      </c>
+      <c r="E11" s="33">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>4</v>
+      </c>
+      <c r="I15" s="5">
+        <v>509</v>
+      </c>
+      <c r="J15" s="5">
+        <v>127.25</v>
+      </c>
+      <c r="K15" s="5">
+        <v>7008.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G16" s="5">
+        <v>2</v>
+      </c>
+      <c r="H16" s="5">
+        <v>4</v>
+      </c>
+      <c r="I16" s="5">
+        <v>3149</v>
+      </c>
+      <c r="J16" s="5">
+        <v>787.25</v>
+      </c>
+      <c r="K16" s="5">
+        <v>57648.25</v>
+      </c>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G17" s="5">
+        <v>3</v>
+      </c>
+      <c r="H17" s="5">
+        <v>4</v>
+      </c>
+      <c r="I17" s="5">
+        <v>203</v>
+      </c>
+      <c r="J17" s="5">
+        <v>50.75</v>
+      </c>
+      <c r="K17" s="5">
+        <v>686.91666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G18" s="5">
+        <v>4</v>
+      </c>
+      <c r="H18" s="5">
+        <v>4</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1586</v>
+      </c>
+      <c r="J18" s="5">
+        <v>396.5</v>
+      </c>
+      <c r="K18" s="5">
+        <v>13663</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G19" s="5">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>4</v>
+      </c>
+      <c r="I19" s="5">
+        <v>856</v>
+      </c>
+      <c r="J19" s="5">
+        <v>214</v>
+      </c>
+      <c r="K19" s="5">
+        <v>10803.333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G20" s="5">
+        <v>6</v>
+      </c>
+      <c r="H20" s="5">
+        <v>4</v>
+      </c>
+      <c r="I20" s="5">
+        <v>762</v>
+      </c>
+      <c r="J20" s="5">
+        <v>190.5</v>
+      </c>
+      <c r="K20" s="5">
+        <v>8257</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G21" s="5">
+        <v>7</v>
+      </c>
+      <c r="H21" s="5">
+        <v>4</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1022</v>
+      </c>
+      <c r="J21" s="5">
+        <v>255.5</v>
+      </c>
+      <c r="K21" s="5">
+        <v>8225</v>
+      </c>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G22" s="5">
+        <v>8</v>
+      </c>
+      <c r="H22" s="5">
+        <v>4</v>
+      </c>
+      <c r="I22" s="5">
+        <v>270</v>
+      </c>
+      <c r="J22" s="5">
+        <v>67.5</v>
+      </c>
+      <c r="K22" s="5">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G23" s="5">
+        <v>9</v>
+      </c>
+      <c r="H23" s="5">
+        <v>4</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1381</v>
+      </c>
+      <c r="J23" s="5">
+        <v>345.25</v>
+      </c>
+      <c r="K23" s="5">
+        <v>3189.5833333333335</v>
+      </c>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G24" s="5">
+        <v>10</v>
+      </c>
+      <c r="H24" s="5">
+        <v>4</v>
+      </c>
+      <c r="I24" s="5">
+        <v>1605</v>
+      </c>
+      <c r="J24" s="5">
+        <v>401.25</v>
+      </c>
+      <c r="K24" s="5">
+        <v>11572.25</v>
+      </c>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G26" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="5">
+        <v>10</v>
+      </c>
+      <c r="I26" s="5">
+        <v>3854</v>
+      </c>
+      <c r="J26" s="5">
+        <v>385.4</v>
+      </c>
+      <c r="K26" s="5">
+        <v>82537.599999999991</v>
+      </c>
+    </row>
+    <row r="27" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G27" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="5">
+        <v>10</v>
+      </c>
+      <c r="I27" s="5">
+        <v>2191</v>
+      </c>
+      <c r="J27" s="5">
+        <v>219.1</v>
+      </c>
+      <c r="K27" s="5">
+        <v>32247.87777777778</v>
+      </c>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G28" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="5">
+        <v>10</v>
+      </c>
+      <c r="I28" s="5">
+        <v>2560</v>
+      </c>
+      <c r="J28" s="5">
+        <v>256</v>
+      </c>
+      <c r="K28" s="5">
+        <v>37373.777777777781</v>
+      </c>
+    </row>
+    <row r="29" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G29" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" s="7">
+        <v>10</v>
+      </c>
+      <c r="I29" s="7">
+        <v>2738</v>
+      </c>
+      <c r="J29" s="7">
+        <v>273.8</v>
+      </c>
+      <c r="K29" s="7">
+        <v>59585.955555555556</v>
+      </c>
+    </row>
+    <row r="32" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G33" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1694868.0249999994</v>
+      </c>
+      <c r="I34" s="5">
+        <v>9</v>
+      </c>
+      <c r="J34" s="5">
+        <v>188318.66944444439</v>
+      </c>
+      <c r="K34" s="5">
+        <v>24.116065289192928</v>
+      </c>
+      <c r="L34" s="5">
+        <v>1.1205167931588805E-10</v>
+      </c>
+      <c r="M34" s="5">
+        <v>3.1493854106511754</v>
+      </c>
+    </row>
+    <row r="35" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G35" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" s="5">
+        <v>153812.87499999953</v>
+      </c>
+      <c r="I35" s="5">
+        <v>3</v>
+      </c>
+      <c r="J35" s="5">
+        <v>51270.958333333176</v>
+      </c>
+      <c r="K35" s="5">
+        <v>6.5657525207341036</v>
+      </c>
+      <c r="L35" s="5">
+        <v>1.7750535652892672E-3</v>
+      </c>
+      <c r="M35" s="5">
+        <v>4.6009068946622849</v>
+      </c>
+    </row>
+    <row r="36" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H36" s="5">
+        <v>210838.87500000047</v>
+      </c>
+      <c r="I36" s="5">
+        <v>27</v>
+      </c>
+      <c r="J36" s="5">
+        <v>7808.8472222222399</v>
+      </c>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" spans="7:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G38" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" s="7">
+        <v>2059519.7749999994</v>
+      </c>
+      <c r="I38" s="7">
+        <v>39</v>
+      </c>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>